<commit_message>
converted calibration pts readings to pd.DF
</commit_message>
<xml_diff>
--- a/use-case-xlsx/calibration-points-template.xlsx
+++ b/use-case-xlsx/calibration-points-template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t xml:space="preserve">Welcome! This sheet provides important information on creation a calibration-points.csv file.</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t xml:space="preserve">Col. 6: Error involved in the measured quantity 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Important: the order of quantities must correspond to the same order defined for ‘Calibration quantity i' in the user input.</t>
   </si>
   <si>
     <t xml:space="preserve">Next, fill in the measurement data in the rows below the header. Every columns must have the same number of rows.</t>
@@ -141,6 +144,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -162,6 +166,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -269,13 +274,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:B31"/>
+  <dimension ref="B2:B32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="111.7"/>
   </cols>
@@ -311,98 +316,103 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="1" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -427,26 +437,26 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -471,26 +481,26 @@
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>